<commit_message>
Finished BOM spreadsheet in design_files.
</commit_message>
<xml_diff>
--- a/design_files/BOM.xlsx
+++ b/design_files/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t xml:space="preserve">Item #</t>
   </si>
@@ -166,7 +166,49 @@
     <t xml:space="preserve">https://www.mcmaster.com/9567K11/</t>
   </si>
   <si>
-    <t xml:space="preserve">not quite done yet</t>
+    <t xml:space="preserve">Black-Oxide 18-8 Pan Head Phillips Screws, M2.5 x 0.45 mm Thread, 10mm Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95836A257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mcmaster.com/95836A257/?SrchEntryWebPart_InpBox=95836A257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steel Thin Hex Nut Medium-Strength, M2.5 x 0.45 mm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">90370A202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mcmaster.com/90370A202/?SrchEntryWebPart_InpBox=95836A257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phillips Screws M3 x 0.50 mm Thread, 20mm Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95836A535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mcmaster.com/95836A535/?SrchEntryWebPart_InpBox=95836A257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hex Nut M3 x 0.5 mm Thread</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98676A100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mcmaster.com/98676A100/?SrchEntryWebPart_InpBox=95836A257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black-Oxide 18-8 Pan Head Phillips Screws M2.5 x 0.45 mm Thread, 20 mm Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95836A216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mcmaster.com/95836A216/?SrchEntryWebPart_InpBox=95836A257</t>
   </si>
   <si>
     <t xml:space="preserve">Note 1</t>
@@ -187,6 +229,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -208,12 +251,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCE181E"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -317,7 +362,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -384,17 +429,17 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="69.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="47.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="67.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="49.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="54.05"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
@@ -647,6 +692,9 @@
       <c r="D10" s="5" t="s">
         <v>42</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F10" s="0" t="s">
         <v>43</v>
       </c>
@@ -670,6 +718,9 @@
       <c r="D11" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="E11" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="F11" s="0" t="s">
         <v>47</v>
       </c>
@@ -680,52 +731,135 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="F12" s="0"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="F13" s="0"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="F14" s="0"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>14</v>
+      </c>
       <c r="B15" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="F15" s="0"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
@@ -779,10 +913,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added missing item to BOM.
</commit_message>
<xml_diff>
--- a/design_files/BOM.xlsx
+++ b/design_files/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t xml:space="preserve">Item #</t>
   </si>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">Heavy Duty Round Caps for 3/4" OD</t>
   </si>
   <si>
-    <t xml:space="preserve">McMaster Carr</t>
+    <t xml:space="preserve">McMaster-Carr</t>
   </si>
   <si>
     <t xml:space="preserve">9567K11</t>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.mcmaster.com/95836A216/?SrchEntryWebPart_InpBox=95836A257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black-Oxide 18-8 Stainless Steel Hex Nut M2.5 x 0.45 mm Thread</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98676A320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mcmaster.com/98676A320/?SrchEntryWebPart_InpBox=98676A320</t>
   </si>
   <si>
     <t xml:space="preserve">Note 1</t>
@@ -345,7 +354,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -429,7 +438,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -861,15 +870,31 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
@@ -913,10 +938,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>